<commit_message>
Fixed one Excel file
</commit_message>
<xml_diff>
--- a/inst/extdata/RP_neg_sample.xlsx
+++ b/inst/extdata/RP_neg_sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Documents\amp\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACD2F55-64EC-4EC1-8222-B5C392523622}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B35D5BC-160A-4C3C-A324-A3103446D0F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1164" yWindow="4272" windowWidth="20244" windowHeight="15984" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18552" yWindow="2868" windowWidth="20244" windowHeight="15984" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RP neg final" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="312">
   <si>
     <t>Class</t>
   </si>
@@ -953,12 +953,6 @@
   </si>
   <si>
     <t>89.922 (100), 36.716 (71), 27.657 (70), 46.402 (59), 80.226 (59), 81.853 (58), 81.37 (55), 84.912 (50), 22.767 (49), 29.27 (49), 45.67 (44), 29.962 (44), 67.84 (43), 48.216 (40), 83.776 (39), 27.905 (32), 74.436 (32), 69.288 (32), 58.727 (30), 40.91 (30), 82.231 (28), 37.642 (27), 84.692 (26), 87.236 (26), 24.544 (22), 35.66 (21), 69.667 (21), 99.491 (20), 52.031 (17), 44.569 (16), 83.098 (14), 87.007 (12), 28.174 (10), 36.311 (9), 81.881 (8), 46.416 (7), 81.386 (6), 22.776 (6), 36.741 (4), 80.265 (4), 40.928 (3), 46.43 (3), 29.302 (3), 27.92 (2), 74.461 (2), 37.677 (2), 89.977 (2), 27.687 (2)</t>
-  </si>
-  <si>
-    <t>100.93464:20711 101.93799:3073 102.94135:1163</t>
-  </si>
-  <si>
-    <t>82.393 (100), 47.397 (96), 66.827 (95), 33.941 (94), 70.852 (93), 50.199 (91), 50.676 (87), 70.348 (81), 83.222 (81), 38.797 (78), 61.457 (75), 43.661 (66), 51.265 (65), 94.108 (65), 38.853 (63), 63.773 (62), 46.23 (60), 26.546 (56), 47.406 (55), 23.238 (52), 50.478 (52), 78.368 (51), 80.607 (47), 41.882 (46), 94.156 (46), 93.84 (46), 55.701 (46), 41.796 (45), 89.007 (44), 85.933 (44), 41.423 (43), 84.948 (43), 50.039 (41), 30.336 (37), 93.999 (36), 69.743 (34), 25.687 (33), 38.719 (32), 49.512 (31), 44.161 (30), 30.563 (28), 66.922 (25), 24.997 (23), 32.691 (21), 27.612 (20), 88.024 (20), 94.407 (19), 25.506 (17), 61.479 (17), 26.279 (17), 41.328 (17), 61.751 (15), 41.145 (13), 36.833 (13), 70.887 (11), 94.129 (10), 47.424 (9), 33.966 (9), 83.247 (8), 51.284 (8), 61.368 (8), 50.697 (7), 49.911 (7), 50.502 (6), 83.26 (6), 66.862 (5), 44.175 (5), 84.979 (5), 82.432 (5), 41.819 (4), 63.798 (4), 38.876 (4), 33.975 (4), 84.971 (4), 43.682 (4), 78.394 (3), 81.569 (3), 50.719 (3), 43.699 (3), 46.25 (3), 57.367 (3), 70.39 (3), 41.441 (2), 46.262 (2), 41.349 (2), 21.038 (2), 50.238 (2), 33.995 (2), 85.968 (2)</t>
   </si>
   <si>
     <t>102.93507:18911 103.93842:0 104.94178:7930</t>
@@ -1803,10 +1797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IH3148"/>
+  <dimension ref="A1:IH3147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="HQ1" workbookViewId="0">
-      <selection activeCell="IE1" sqref="IE1:IF1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18197,25 +18191,25 @@
     </row>
     <row r="24" spans="1:242" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B24">
-        <v>15.52</v>
+        <v>15.37</v>
       </c>
       <c r="C24">
-        <v>100.9346</v>
+        <v>102.9355</v>
       </c>
       <c r="D24" t="s">
         <v>257</v>
       </c>
       <c r="E24" t="s">
-        <v>306</v>
+        <v>252</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>0.8475336</v>
       </c>
       <c r="H24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" t="s">
         <v>258</v>
@@ -18245,1439 +18239,1389 @@
         <v>-1</v>
       </c>
       <c r="S24" t="s">
-        <v>248</v>
+        <v>89</v>
       </c>
       <c r="T24" t="s">
         <v>311</v>
       </c>
-      <c r="U24" t="s">
-        <v>312</v>
+      <c r="V24">
+        <v>14987.76</v>
+      </c>
+      <c r="W24">
+        <v>36568.97</v>
+      </c>
+      <c r="X24">
+        <v>23433.83</v>
+      </c>
+      <c r="Y24">
+        <v>29355.42</v>
+      </c>
+      <c r="Z24">
+        <v>26189.13</v>
+      </c>
+      <c r="AA24">
+        <v>4860.8609999999999</v>
+      </c>
+      <c r="AB24">
+        <v>42219.02</v>
+      </c>
+      <c r="AC24">
+        <v>1975.855</v>
+      </c>
+      <c r="AD24">
+        <v>36019.660000000003</v>
+      </c>
+      <c r="AE24">
+        <v>108125</v>
+      </c>
+      <c r="AF24">
+        <v>47725.34</v>
+      </c>
+      <c r="AG24">
+        <v>23763.64</v>
+      </c>
+      <c r="AH24">
+        <v>28072.5</v>
+      </c>
+      <c r="AI24">
+        <v>19771.96</v>
+      </c>
+      <c r="AJ24">
+        <v>31607.83</v>
+      </c>
+      <c r="AK24">
+        <v>36085.919999999998</v>
+      </c>
+      <c r="AL24">
+        <v>38033.22</v>
+      </c>
+      <c r="AM24">
+        <v>30992.75</v>
+      </c>
+      <c r="AN24">
+        <v>24948.17</v>
+      </c>
+      <c r="AO24">
+        <v>41628.81</v>
+      </c>
+      <c r="AP24">
+        <v>27711.85</v>
+      </c>
+      <c r="AQ24">
+        <v>22196.37</v>
+      </c>
+      <c r="AR24">
+        <v>37407.269999999997</v>
+      </c>
+      <c r="AS24">
+        <v>23183.599999999999</v>
+      </c>
+      <c r="AT24">
+        <v>24311.05</v>
+      </c>
+      <c r="AU24">
+        <v>37321.160000000003</v>
+      </c>
+      <c r="AV24">
+        <v>11977.48</v>
+      </c>
+      <c r="AW24">
+        <v>31376.76</v>
+      </c>
+      <c r="AX24">
+        <v>260885.6</v>
+      </c>
+      <c r="AY24">
+        <v>22223.49</v>
+      </c>
+      <c r="AZ24">
+        <v>84514.22</v>
+      </c>
+      <c r="BA24">
+        <v>22760</v>
+      </c>
+      <c r="BB24">
+        <v>30963.14</v>
+      </c>
+      <c r="BC24">
+        <v>32461.49</v>
+      </c>
+      <c r="BD24">
+        <v>26027.17</v>
+      </c>
+      <c r="BE24">
+        <v>23953.34</v>
+      </c>
+      <c r="BF24">
+        <v>80680.58</v>
+      </c>
+      <c r="BG24">
+        <v>38171</v>
+      </c>
+      <c r="BH24">
+        <v>34161.339999999997</v>
+      </c>
+      <c r="BI24">
+        <v>22493.34</v>
+      </c>
+      <c r="BJ24">
+        <v>23682.81</v>
+      </c>
+      <c r="BK24">
+        <v>33604.49</v>
+      </c>
+      <c r="BL24">
+        <v>1145.5409999999999</v>
+      </c>
+      <c r="BM24">
+        <v>35238.33</v>
+      </c>
+      <c r="BN24">
+        <v>35436.300000000003</v>
+      </c>
+      <c r="BO24">
+        <v>24794.53</v>
+      </c>
+      <c r="BP24">
+        <v>36818.080000000002</v>
+      </c>
+      <c r="BQ24">
+        <v>33106.449999999997</v>
+      </c>
+      <c r="BR24">
+        <v>30412.54</v>
+      </c>
+      <c r="BS24">
+        <v>37080.11</v>
+      </c>
+      <c r="BT24">
+        <v>54852.09</v>
+      </c>
+      <c r="BU24">
+        <v>20357.04</v>
+      </c>
+      <c r="BV24">
+        <v>18829.72</v>
+      </c>
+      <c r="BW24">
+        <v>40606.35</v>
+      </c>
+      <c r="BX24">
+        <v>37960.18</v>
+      </c>
+      <c r="BY24">
+        <v>29696.12</v>
+      </c>
+      <c r="BZ24">
+        <v>17868.91</v>
+      </c>
+      <c r="CA24">
+        <v>36587.910000000003</v>
+      </c>
+      <c r="CB24">
+        <v>31228.67</v>
+      </c>
+      <c r="CC24">
+        <v>37232.65</v>
+      </c>
+      <c r="CD24">
+        <v>20202.810000000001</v>
+      </c>
+      <c r="CE24">
+        <v>20021.32</v>
+      </c>
+      <c r="CF24">
+        <v>27520.65</v>
+      </c>
+      <c r="CG24">
+        <v>53412.58</v>
+      </c>
+      <c r="CH24">
+        <v>24125.11</v>
+      </c>
+      <c r="CI24">
+        <v>19469.810000000001</v>
+      </c>
+      <c r="CJ24">
+        <v>22467.87</v>
+      </c>
+      <c r="CK24">
+        <v>22102.79</v>
+      </c>
+      <c r="CL24">
+        <v>33115.5</v>
+      </c>
+      <c r="CM24">
+        <v>35596.959999999999</v>
+      </c>
+      <c r="CN24">
+        <v>20240.599999999999</v>
+      </c>
+      <c r="CO24">
+        <v>35184.9</v>
+      </c>
+      <c r="CP24">
+        <v>34241.730000000003</v>
+      </c>
+      <c r="CQ24">
+        <v>35000.980000000003</v>
+      </c>
+      <c r="CR24">
+        <v>37447.64</v>
+      </c>
+      <c r="CS24">
+        <v>24846.34</v>
+      </c>
+      <c r="CT24">
+        <v>23411.4</v>
+      </c>
+      <c r="CU24">
+        <v>107605.3</v>
+      </c>
+      <c r="CV24">
+        <v>25202.32</v>
+      </c>
+      <c r="CW24">
+        <v>43916.21</v>
+      </c>
+      <c r="CX24">
+        <v>182341.4</v>
+      </c>
+      <c r="CY24">
+        <v>40136.589999999997</v>
+      </c>
+      <c r="CZ24">
+        <v>108902.7</v>
+      </c>
+      <c r="DA24">
+        <v>20186.53</v>
+      </c>
+      <c r="DB24">
+        <v>21241.79</v>
+      </c>
+      <c r="DC24">
+        <v>21520.97</v>
+      </c>
+      <c r="DD24">
+        <v>32461.88</v>
+      </c>
+      <c r="DE24">
+        <v>32492.95</v>
+      </c>
+      <c r="DF24">
+        <v>41234.01</v>
+      </c>
+      <c r="DG24">
+        <v>23364.46</v>
+      </c>
+      <c r="DH24">
+        <v>25196.53</v>
+      </c>
+      <c r="DI24">
+        <v>23839.16</v>
+      </c>
+      <c r="DJ24">
+        <v>109704.6</v>
+      </c>
+      <c r="DK24">
+        <v>179295.7</v>
+      </c>
+      <c r="DL24">
+        <v>45959.360000000001</v>
+      </c>
+      <c r="DM24">
+        <v>79246.48</v>
+      </c>
+      <c r="DN24">
+        <v>28971.74</v>
+      </c>
+      <c r="DO24">
+        <v>100284.4</v>
+      </c>
+      <c r="DP24">
+        <v>26021.47</v>
+      </c>
+      <c r="DQ24">
+        <v>34868.86</v>
+      </c>
+      <c r="DR24">
+        <v>31155.040000000001</v>
+      </c>
+      <c r="DS24">
+        <v>37050.379999999997</v>
+      </c>
+      <c r="DT24">
+        <v>31756.97</v>
+      </c>
+      <c r="DU24">
+        <v>46932.21</v>
+      </c>
+      <c r="DV24">
+        <v>28598.27</v>
+      </c>
+      <c r="DW24">
+        <v>30620.87</v>
+      </c>
+      <c r="DX24">
+        <v>29398.400000000001</v>
+      </c>
+      <c r="DY24">
+        <v>30979.78</v>
+      </c>
+      <c r="DZ24">
+        <v>26740.75</v>
+      </c>
+      <c r="EA24">
+        <v>22907.11</v>
+      </c>
+      <c r="EB24">
+        <v>26544.06</v>
+      </c>
+      <c r="EC24">
+        <v>27814.74</v>
+      </c>
+      <c r="ED24">
+        <v>23073.360000000001</v>
+      </c>
+      <c r="EE24">
+        <v>29931.82</v>
+      </c>
+      <c r="EF24">
+        <v>48440.79</v>
+      </c>
+      <c r="EG24">
+        <v>36311.57</v>
+      </c>
+      <c r="EH24">
+        <v>28425</v>
+      </c>
+      <c r="EI24">
+        <v>23682.11</v>
+      </c>
+      <c r="EJ24">
+        <v>34699.9</v>
+      </c>
+      <c r="EK24">
+        <v>32002.48</v>
+      </c>
+      <c r="EL24">
+        <v>166922.70000000001</v>
+      </c>
+      <c r="EM24">
+        <v>19488.38</v>
+      </c>
+      <c r="EN24">
+        <v>31948.85</v>
+      </c>
+      <c r="EO24">
+        <v>22574.62</v>
+      </c>
+      <c r="EP24">
+        <v>32807.589999999997</v>
+      </c>
+      <c r="EQ24">
+        <v>20654.599999999999</v>
+      </c>
+      <c r="ER24">
+        <v>38952.92</v>
+      </c>
+      <c r="ES24">
+        <v>14466.34</v>
+      </c>
+      <c r="ET24">
+        <v>118607.9</v>
+      </c>
+      <c r="EU24">
+        <v>96057.96</v>
+      </c>
+      <c r="EV24">
+        <v>24383.22</v>
+      </c>
+      <c r="EW24">
+        <v>33348.39</v>
+      </c>
+      <c r="EX24">
+        <v>26284.32</v>
+      </c>
+      <c r="EY24">
+        <v>34547.56</v>
+      </c>
+      <c r="EZ24">
+        <v>27449.08</v>
+      </c>
+      <c r="FA24">
+        <v>106565.8</v>
+      </c>
+      <c r="FB24">
+        <v>13338.12</v>
+      </c>
+      <c r="FC24">
+        <v>23171.51</v>
+      </c>
+      <c r="FD24">
+        <v>12877.29</v>
+      </c>
+      <c r="FE24">
+        <v>23153.439999999999</v>
+      </c>
+      <c r="FF24">
+        <v>25691.09</v>
+      </c>
+      <c r="FG24">
+        <v>32207.4</v>
+      </c>
+      <c r="FH24">
+        <v>90830.58</v>
+      </c>
+      <c r="FI24">
+        <v>19277.39</v>
+      </c>
+      <c r="FJ24">
+        <v>20989.41</v>
+      </c>
+      <c r="FK24">
+        <v>42115.99</v>
+      </c>
+      <c r="FL24">
+        <v>27826.46</v>
+      </c>
+      <c r="FM24">
+        <v>14942.49</v>
+      </c>
+      <c r="FN24">
+        <v>24345.85</v>
+      </c>
+      <c r="FO24">
+        <v>31078.92</v>
+      </c>
+      <c r="FP24">
+        <v>24571.71</v>
+      </c>
+      <c r="FQ24">
+        <v>24455.63</v>
+      </c>
+      <c r="FR24">
+        <v>23317.87</v>
+      </c>
+      <c r="FS24">
+        <v>48461.58</v>
+      </c>
+      <c r="FT24">
+        <v>25623.38</v>
+      </c>
+      <c r="FU24">
+        <v>23992.9</v>
+      </c>
+      <c r="FV24">
+        <v>26226.29</v>
+      </c>
+      <c r="FW24">
+        <v>31048.07</v>
+      </c>
+      <c r="FX24">
+        <v>43497.71</v>
+      </c>
+      <c r="FY24">
+        <v>28093.17</v>
+      </c>
+      <c r="FZ24">
+        <v>16085.61</v>
+      </c>
+      <c r="GA24">
+        <v>161795</v>
+      </c>
+      <c r="GB24">
+        <v>634.69389999999999</v>
+      </c>
+      <c r="GC24">
+        <v>23738.48</v>
+      </c>
+      <c r="GD24">
+        <v>27566.74</v>
+      </c>
+      <c r="GE24">
+        <v>1540.086</v>
+      </c>
+      <c r="GF24">
+        <v>23735.360000000001</v>
+      </c>
+      <c r="GG24">
+        <v>23489.46</v>
+      </c>
+      <c r="GH24">
+        <v>4916.7380000000003</v>
+      </c>
+      <c r="GI24">
+        <v>34281.46</v>
+      </c>
+      <c r="GJ24">
+        <v>27310.799999999999</v>
+      </c>
+      <c r="GK24">
+        <v>22050.43</v>
+      </c>
+      <c r="GL24">
+        <v>28884.34</v>
+      </c>
+      <c r="GM24">
+        <v>93779.23</v>
+      </c>
+      <c r="GN24">
+        <v>27869.87</v>
+      </c>
+      <c r="GO24">
+        <v>90463.01</v>
+      </c>
+      <c r="GP24">
+        <v>23774.33</v>
+      </c>
+      <c r="GQ24">
+        <v>24883.22</v>
+      </c>
+      <c r="GR24">
+        <v>17780.060000000001</v>
+      </c>
+      <c r="GS24">
+        <v>17502.23</v>
+      </c>
+      <c r="GT24">
+        <v>15118.25</v>
+      </c>
+      <c r="GU24">
+        <v>15641.38</v>
+      </c>
+      <c r="GV24">
+        <v>25303.11</v>
+      </c>
+      <c r="GW24">
+        <v>30733.83</v>
+      </c>
+      <c r="GX24">
+        <v>30944.400000000001</v>
+      </c>
+      <c r="GY24">
+        <v>19682.189999999999</v>
+      </c>
+      <c r="GZ24">
+        <v>17335.62</v>
+      </c>
+      <c r="HA24">
+        <v>30831.87</v>
+      </c>
+      <c r="HB24">
+        <v>27257.46</v>
+      </c>
+      <c r="HC24">
+        <v>29796.720000000001</v>
+      </c>
+      <c r="HD24">
+        <v>39144.160000000003</v>
+      </c>
+      <c r="HE24">
+        <v>32590.89</v>
+      </c>
+      <c r="HF24">
+        <v>29929.119999999999</v>
+      </c>
+      <c r="HG24">
+        <v>29884.44</v>
+      </c>
+      <c r="HH24">
+        <v>27028.25</v>
+      </c>
+      <c r="HI24">
+        <v>21350.55</v>
+      </c>
+      <c r="HJ24">
+        <v>1767.31</v>
+      </c>
+      <c r="HK24">
+        <v>22191.5</v>
+      </c>
+      <c r="HL24">
+        <v>45829.68</v>
+      </c>
+      <c r="HM24">
+        <v>16926.189999999999</v>
+      </c>
+      <c r="HN24">
+        <v>22944.39</v>
+      </c>
+      <c r="HO24">
+        <v>28106.94</v>
+      </c>
+      <c r="HP24">
+        <v>22951.5</v>
+      </c>
+      <c r="HQ24">
+        <v>19737.73</v>
+      </c>
+      <c r="HR24">
+        <v>33721.82</v>
+      </c>
+      <c r="HS24">
+        <v>29944.46</v>
+      </c>
+      <c r="HT24">
+        <v>32627.17</v>
+      </c>
+      <c r="HU24">
+        <v>32555.86</v>
+      </c>
+      <c r="HV24">
+        <v>26982.09</v>
+      </c>
+      <c r="HW24">
+        <v>31393.68</v>
+      </c>
+      <c r="HX24">
+        <v>30433.19</v>
+      </c>
+      <c r="HY24">
+        <v>104504.7</v>
+      </c>
+      <c r="HZ24">
+        <v>34883.9</v>
+      </c>
+      <c r="IA24">
+        <v>38205.550000000003</v>
+      </c>
+      <c r="IB24">
+        <v>81405.41</v>
+      </c>
+      <c r="IC24">
+        <v>30856.39</v>
+      </c>
+      <c r="ID24">
+        <v>20505.5</v>
+      </c>
+      <c r="IE24">
+        <v>24102.13</v>
+      </c>
+      <c r="IF24">
+        <v>22250.97</v>
+      </c>
+      <c r="IG24">
+        <v>6798.0309999999999</v>
+      </c>
+      <c r="IH24">
+        <v>24050.639999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:242" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>20</v>
-      </c>
-      <c r="B25">
-        <v>15.37</v>
-      </c>
-      <c r="C25">
-        <v>102.9355</v>
-      </c>
-      <c r="D25" t="s">
-        <v>257</v>
-      </c>
-      <c r="E25" t="s">
-        <v>252</v>
-      </c>
-      <c r="G25">
-        <v>0.8475336</v>
-      </c>
-      <c r="H25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I25" t="s">
-        <v>258</v>
-      </c>
-      <c r="J25" t="s">
-        <v>258</v>
-      </c>
-      <c r="K25" t="s">
-        <v>258</v>
-      </c>
-      <c r="L25" t="s">
-        <v>258</v>
-      </c>
-      <c r="N25">
-        <v>-1</v>
-      </c>
-      <c r="O25">
-        <v>-1</v>
-      </c>
-      <c r="P25">
-        <v>-1</v>
-      </c>
-      <c r="Q25">
-        <v>-1</v>
-      </c>
-      <c r="R25">
-        <v>-1</v>
-      </c>
-      <c r="S25" t="s">
-        <v>89</v>
-      </c>
-      <c r="T25" t="s">
-        <v>313</v>
-      </c>
-      <c r="V25">
-        <v>14987.76</v>
-      </c>
-      <c r="W25">
-        <v>36568.97</v>
-      </c>
-      <c r="X25">
-        <v>23433.83</v>
-      </c>
-      <c r="Y25">
-        <v>29355.42</v>
-      </c>
-      <c r="Z25">
-        <v>26189.13</v>
-      </c>
-      <c r="AA25">
-        <v>4860.8609999999999</v>
-      </c>
-      <c r="AB25">
-        <v>42219.02</v>
-      </c>
-      <c r="AC25">
-        <v>1975.855</v>
-      </c>
-      <c r="AD25">
-        <v>36019.660000000003</v>
-      </c>
-      <c r="AE25">
-        <v>108125</v>
-      </c>
-      <c r="AF25">
-        <v>47725.34</v>
-      </c>
-      <c r="AG25">
-        <v>23763.64</v>
-      </c>
-      <c r="AH25">
-        <v>28072.5</v>
-      </c>
-      <c r="AI25">
-        <v>19771.96</v>
-      </c>
-      <c r="AJ25">
-        <v>31607.83</v>
-      </c>
-      <c r="AK25">
-        <v>36085.919999999998</v>
-      </c>
-      <c r="AL25">
-        <v>38033.22</v>
-      </c>
-      <c r="AM25">
-        <v>30992.75</v>
-      </c>
-      <c r="AN25">
-        <v>24948.17</v>
-      </c>
-      <c r="AO25">
-        <v>41628.81</v>
-      </c>
-      <c r="AP25">
-        <v>27711.85</v>
-      </c>
-      <c r="AQ25">
-        <v>22196.37</v>
-      </c>
-      <c r="AR25">
-        <v>37407.269999999997</v>
-      </c>
-      <c r="AS25">
-        <v>23183.599999999999</v>
-      </c>
-      <c r="AT25">
-        <v>24311.05</v>
-      </c>
-      <c r="AU25">
-        <v>37321.160000000003</v>
-      </c>
-      <c r="AV25">
-        <v>11977.48</v>
-      </c>
-      <c r="AW25">
-        <v>31376.76</v>
-      </c>
-      <c r="AX25">
-        <v>260885.6</v>
-      </c>
-      <c r="AY25">
-        <v>22223.49</v>
-      </c>
-      <c r="AZ25">
-        <v>84514.22</v>
-      </c>
-      <c r="BA25">
-        <v>22760</v>
-      </c>
-      <c r="BB25">
-        <v>30963.14</v>
-      </c>
-      <c r="BC25">
-        <v>32461.49</v>
-      </c>
-      <c r="BD25">
-        <v>26027.17</v>
-      </c>
-      <c r="BE25">
-        <v>23953.34</v>
-      </c>
-      <c r="BF25">
-        <v>80680.58</v>
-      </c>
-      <c r="BG25">
-        <v>38171</v>
-      </c>
-      <c r="BH25">
-        <v>34161.339999999997</v>
-      </c>
-      <c r="BI25">
-        <v>22493.34</v>
-      </c>
-      <c r="BJ25">
-        <v>23682.81</v>
-      </c>
-      <c r="BK25">
-        <v>33604.49</v>
-      </c>
-      <c r="BL25">
-        <v>1145.5409999999999</v>
-      </c>
-      <c r="BM25">
-        <v>35238.33</v>
-      </c>
-      <c r="BN25">
-        <v>35436.300000000003</v>
-      </c>
-      <c r="BO25">
-        <v>24794.53</v>
-      </c>
-      <c r="BP25">
-        <v>36818.080000000002</v>
-      </c>
-      <c r="BQ25">
-        <v>33106.449999999997</v>
-      </c>
-      <c r="BR25">
-        <v>30412.54</v>
-      </c>
-      <c r="BS25">
-        <v>37080.11</v>
-      </c>
-      <c r="BT25">
-        <v>54852.09</v>
-      </c>
-      <c r="BU25">
-        <v>20357.04</v>
-      </c>
-      <c r="BV25">
-        <v>18829.72</v>
-      </c>
-      <c r="BW25">
-        <v>40606.35</v>
-      </c>
-      <c r="BX25">
-        <v>37960.18</v>
-      </c>
-      <c r="BY25">
-        <v>29696.12</v>
-      </c>
-      <c r="BZ25">
-        <v>17868.91</v>
-      </c>
-      <c r="CA25">
-        <v>36587.910000000003</v>
-      </c>
-      <c r="CB25">
-        <v>31228.67</v>
-      </c>
-      <c r="CC25">
-        <v>37232.65</v>
-      </c>
-      <c r="CD25">
-        <v>20202.810000000001</v>
-      </c>
-      <c r="CE25">
-        <v>20021.32</v>
-      </c>
-      <c r="CF25">
-        <v>27520.65</v>
-      </c>
-      <c r="CG25">
-        <v>53412.58</v>
-      </c>
-      <c r="CH25">
-        <v>24125.11</v>
-      </c>
-      <c r="CI25">
-        <v>19469.810000000001</v>
-      </c>
-      <c r="CJ25">
-        <v>22467.87</v>
-      </c>
-      <c r="CK25">
-        <v>22102.79</v>
-      </c>
-      <c r="CL25">
-        <v>33115.5</v>
-      </c>
-      <c r="CM25">
-        <v>35596.959999999999</v>
-      </c>
-      <c r="CN25">
-        <v>20240.599999999999</v>
-      </c>
-      <c r="CO25">
-        <v>35184.9</v>
-      </c>
-      <c r="CP25">
-        <v>34241.730000000003</v>
-      </c>
-      <c r="CQ25">
-        <v>35000.980000000003</v>
-      </c>
-      <c r="CR25">
-        <v>37447.64</v>
-      </c>
-      <c r="CS25">
-        <v>24846.34</v>
-      </c>
-      <c r="CT25">
-        <v>23411.4</v>
-      </c>
-      <c r="CU25">
-        <v>107605.3</v>
-      </c>
-      <c r="CV25">
-        <v>25202.32</v>
-      </c>
-      <c r="CW25">
-        <v>43916.21</v>
-      </c>
-      <c r="CX25">
-        <v>182341.4</v>
-      </c>
-      <c r="CY25">
-        <v>40136.589999999997</v>
-      </c>
-      <c r="CZ25">
-        <v>108902.7</v>
-      </c>
-      <c r="DA25">
-        <v>20186.53</v>
-      </c>
-      <c r="DB25">
-        <v>21241.79</v>
-      </c>
-      <c r="DC25">
-        <v>21520.97</v>
-      </c>
-      <c r="DD25">
-        <v>32461.88</v>
-      </c>
-      <c r="DE25">
-        <v>32492.95</v>
-      </c>
-      <c r="DF25">
-        <v>41234.01</v>
-      </c>
-      <c r="DG25">
-        <v>23364.46</v>
-      </c>
-      <c r="DH25">
-        <v>25196.53</v>
-      </c>
-      <c r="DI25">
-        <v>23839.16</v>
-      </c>
-      <c r="DJ25">
-        <v>109704.6</v>
-      </c>
-      <c r="DK25">
-        <v>179295.7</v>
-      </c>
-      <c r="DL25">
-        <v>45959.360000000001</v>
-      </c>
-      <c r="DM25">
-        <v>79246.48</v>
-      </c>
-      <c r="DN25">
-        <v>28971.74</v>
-      </c>
-      <c r="DO25">
-        <v>100284.4</v>
-      </c>
-      <c r="DP25">
-        <v>26021.47</v>
-      </c>
-      <c r="DQ25">
-        <v>34868.86</v>
-      </c>
-      <c r="DR25">
-        <v>31155.040000000001</v>
-      </c>
-      <c r="DS25">
-        <v>37050.379999999997</v>
-      </c>
-      <c r="DT25">
-        <v>31756.97</v>
-      </c>
-      <c r="DU25">
-        <v>46932.21</v>
-      </c>
-      <c r="DV25">
-        <v>28598.27</v>
-      </c>
-      <c r="DW25">
-        <v>30620.87</v>
-      </c>
-      <c r="DX25">
-        <v>29398.400000000001</v>
-      </c>
-      <c r="DY25">
-        <v>30979.78</v>
-      </c>
-      <c r="DZ25">
-        <v>26740.75</v>
-      </c>
-      <c r="EA25">
-        <v>22907.11</v>
-      </c>
-      <c r="EB25">
-        <v>26544.06</v>
-      </c>
-      <c r="EC25">
-        <v>27814.74</v>
-      </c>
-      <c r="ED25">
-        <v>23073.360000000001</v>
-      </c>
-      <c r="EE25">
-        <v>29931.82</v>
-      </c>
-      <c r="EF25">
-        <v>48440.79</v>
-      </c>
-      <c r="EG25">
-        <v>36311.57</v>
-      </c>
-      <c r="EH25">
-        <v>28425</v>
-      </c>
-      <c r="EI25">
-        <v>23682.11</v>
-      </c>
-      <c r="EJ25">
-        <v>34699.9</v>
-      </c>
-      <c r="EK25">
-        <v>32002.48</v>
-      </c>
-      <c r="EL25">
-        <v>166922.70000000001</v>
-      </c>
-      <c r="EM25">
-        <v>19488.38</v>
-      </c>
-      <c r="EN25">
-        <v>31948.85</v>
-      </c>
-      <c r="EO25">
-        <v>22574.62</v>
-      </c>
-      <c r="EP25">
-        <v>32807.589999999997</v>
-      </c>
-      <c r="EQ25">
-        <v>20654.599999999999</v>
-      </c>
-      <c r="ER25">
-        <v>38952.92</v>
-      </c>
-      <c r="ES25">
-        <v>14466.34</v>
-      </c>
-      <c r="ET25">
-        <v>118607.9</v>
-      </c>
-      <c r="EU25">
-        <v>96057.96</v>
-      </c>
-      <c r="EV25">
-        <v>24383.22</v>
-      </c>
-      <c r="EW25">
-        <v>33348.39</v>
-      </c>
-      <c r="EX25">
-        <v>26284.32</v>
-      </c>
-      <c r="EY25">
-        <v>34547.56</v>
-      </c>
-      <c r="EZ25">
-        <v>27449.08</v>
-      </c>
-      <c r="FA25">
-        <v>106565.8</v>
-      </c>
-      <c r="FB25">
-        <v>13338.12</v>
-      </c>
-      <c r="FC25">
-        <v>23171.51</v>
-      </c>
-      <c r="FD25">
-        <v>12877.29</v>
-      </c>
-      <c r="FE25">
-        <v>23153.439999999999</v>
-      </c>
-      <c r="FF25">
-        <v>25691.09</v>
-      </c>
-      <c r="FG25">
-        <v>32207.4</v>
-      </c>
-      <c r="FH25">
-        <v>90830.58</v>
-      </c>
-      <c r="FI25">
-        <v>19277.39</v>
-      </c>
-      <c r="FJ25">
-        <v>20989.41</v>
-      </c>
-      <c r="FK25">
-        <v>42115.99</v>
-      </c>
-      <c r="FL25">
-        <v>27826.46</v>
-      </c>
-      <c r="FM25">
-        <v>14942.49</v>
-      </c>
-      <c r="FN25">
-        <v>24345.85</v>
-      </c>
-      <c r="FO25">
-        <v>31078.92</v>
-      </c>
-      <c r="FP25">
-        <v>24571.71</v>
-      </c>
-      <c r="FQ25">
-        <v>24455.63</v>
-      </c>
-      <c r="FR25">
-        <v>23317.87</v>
-      </c>
-      <c r="FS25">
-        <v>48461.58</v>
-      </c>
-      <c r="FT25">
-        <v>25623.38</v>
-      </c>
-      <c r="FU25">
-        <v>23992.9</v>
-      </c>
-      <c r="FV25">
-        <v>26226.29</v>
-      </c>
-      <c r="FW25">
-        <v>31048.07</v>
-      </c>
-      <c r="FX25">
-        <v>43497.71</v>
-      </c>
-      <c r="FY25">
-        <v>28093.17</v>
-      </c>
-      <c r="FZ25">
-        <v>16085.61</v>
-      </c>
-      <c r="GA25">
-        <v>161795</v>
-      </c>
-      <c r="GB25">
-        <v>634.69389999999999</v>
-      </c>
-      <c r="GC25">
-        <v>23738.48</v>
-      </c>
-      <c r="GD25">
-        <v>27566.74</v>
-      </c>
-      <c r="GE25">
-        <v>1540.086</v>
-      </c>
-      <c r="GF25">
-        <v>23735.360000000001</v>
-      </c>
-      <c r="GG25">
-        <v>23489.46</v>
-      </c>
-      <c r="GH25">
-        <v>4916.7380000000003</v>
-      </c>
-      <c r="GI25">
-        <v>34281.46</v>
-      </c>
-      <c r="GJ25">
-        <v>27310.799999999999</v>
-      </c>
-      <c r="GK25">
-        <v>22050.43</v>
-      </c>
-      <c r="GL25">
-        <v>28884.34</v>
-      </c>
-      <c r="GM25">
-        <v>93779.23</v>
-      </c>
-      <c r="GN25">
-        <v>27869.87</v>
-      </c>
-      <c r="GO25">
-        <v>90463.01</v>
-      </c>
-      <c r="GP25">
-        <v>23774.33</v>
-      </c>
-      <c r="GQ25">
-        <v>24883.22</v>
-      </c>
-      <c r="GR25">
-        <v>17780.060000000001</v>
-      </c>
-      <c r="GS25">
-        <v>17502.23</v>
-      </c>
-      <c r="GT25">
-        <v>15118.25</v>
-      </c>
-      <c r="GU25">
-        <v>15641.38</v>
-      </c>
-      <c r="GV25">
-        <v>25303.11</v>
-      </c>
-      <c r="GW25">
-        <v>30733.83</v>
-      </c>
-      <c r="GX25">
-        <v>30944.400000000001</v>
-      </c>
-      <c r="GY25">
-        <v>19682.189999999999</v>
-      </c>
-      <c r="GZ25">
-        <v>17335.62</v>
-      </c>
-      <c r="HA25">
-        <v>30831.87</v>
-      </c>
-      <c r="HB25">
-        <v>27257.46</v>
-      </c>
-      <c r="HC25">
-        <v>29796.720000000001</v>
-      </c>
-      <c r="HD25">
-        <v>39144.160000000003</v>
-      </c>
-      <c r="HE25">
-        <v>32590.89</v>
-      </c>
-      <c r="HF25">
-        <v>29929.119999999999</v>
-      </c>
-      <c r="HG25">
-        <v>29884.44</v>
-      </c>
-      <c r="HH25">
-        <v>27028.25</v>
-      </c>
-      <c r="HI25">
-        <v>21350.55</v>
-      </c>
-      <c r="HJ25">
-        <v>1767.31</v>
-      </c>
-      <c r="HK25">
-        <v>22191.5</v>
-      </c>
-      <c r="HL25">
-        <v>45829.68</v>
-      </c>
-      <c r="HM25">
-        <v>16926.189999999999</v>
-      </c>
-      <c r="HN25">
-        <v>22944.39</v>
-      </c>
-      <c r="HO25">
-        <v>28106.94</v>
-      </c>
-      <c r="HP25">
-        <v>22951.5</v>
-      </c>
-      <c r="HQ25">
-        <v>19737.73</v>
-      </c>
-      <c r="HR25">
-        <v>33721.82</v>
-      </c>
-      <c r="HS25">
-        <v>29944.46</v>
-      </c>
-      <c r="HT25">
-        <v>32627.17</v>
-      </c>
-      <c r="HU25">
-        <v>32555.86</v>
-      </c>
-      <c r="HV25">
-        <v>26982.09</v>
-      </c>
-      <c r="HW25">
-        <v>31393.68</v>
-      </c>
-      <c r="HX25">
-        <v>30433.19</v>
-      </c>
-      <c r="HY25">
-        <v>104504.7</v>
-      </c>
-      <c r="HZ25">
-        <v>34883.9</v>
-      </c>
-      <c r="IA25">
-        <v>38205.550000000003</v>
-      </c>
-      <c r="IB25">
-        <v>81405.41</v>
-      </c>
-      <c r="IC25">
-        <v>30856.39</v>
-      </c>
-      <c r="ID25">
-        <v>20505.5</v>
-      </c>
-      <c r="IE25">
-        <v>24102.13</v>
-      </c>
-      <c r="IF25">
-        <v>22250.97</v>
-      </c>
-      <c r="IG25">
-        <v>6798.0309999999999</v>
-      </c>
-      <c r="IH25">
-        <v>24050.639999999999</v>
-      </c>
+    <row r="39" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA39" s="1"/>
     </row>
-    <row r="40" spans="27:27" x14ac:dyDescent="0.3">
-      <c r="AA40" s="1"/>
+    <row r="160" spans="187:187" x14ac:dyDescent="0.3">
+      <c r="GE160" s="1"/>
     </row>
-    <row r="161" spans="187:187" x14ac:dyDescent="0.3">
-      <c r="GE161" s="1"/>
+    <row r="182" spans="112:145" x14ac:dyDescent="0.3">
+      <c r="DH182" s="1"/>
+      <c r="EO182" s="1"/>
     </row>
-    <row r="183" spans="112:145" x14ac:dyDescent="0.3">
-      <c r="DH183" s="1"/>
-      <c r="EO183" s="1"/>
+    <row r="201" spans="27:236" x14ac:dyDescent="0.3">
+      <c r="AA201" s="1"/>
+      <c r="AC201" s="1"/>
+      <c r="AT201" s="1"/>
+      <c r="BL201" s="1"/>
+      <c r="GE201" s="1"/>
+      <c r="HZ201" s="1"/>
+      <c r="IB201" s="1"/>
     </row>
-    <row r="202" spans="27:236" x14ac:dyDescent="0.3">
-      <c r="AA202" s="1"/>
-      <c r="AC202" s="1"/>
-      <c r="AT202" s="1"/>
-      <c r="BL202" s="1"/>
-      <c r="GE202" s="1"/>
-      <c r="HZ202" s="1"/>
-      <c r="IB202" s="1"/>
+    <row r="375" spans="30:238" x14ac:dyDescent="0.3">
+      <c r="AD375" s="1"/>
+      <c r="AE375" s="1"/>
+      <c r="AF375" s="1"/>
+      <c r="AJ375" s="1"/>
+      <c r="AP375" s="1"/>
+      <c r="AQ375" s="1"/>
+      <c r="AT375" s="1"/>
+      <c r="AU375" s="1"/>
+      <c r="AX375" s="1"/>
+      <c r="AZ375" s="1"/>
+      <c r="BA375" s="1"/>
+      <c r="BB375" s="1"/>
+      <c r="BD375" s="1"/>
+      <c r="BF375" s="1"/>
+      <c r="BG375" s="1"/>
+      <c r="BH375" s="1"/>
+      <c r="BJ375" s="1"/>
+      <c r="BK375" s="1"/>
+      <c r="BM375" s="1"/>
+      <c r="BN375" s="1"/>
+      <c r="BO375" s="1"/>
+      <c r="BR375" s="1"/>
+      <c r="BT375" s="1"/>
+      <c r="BU375" s="1"/>
+      <c r="BV375" s="1"/>
+      <c r="BW375" s="1"/>
+      <c r="BX375" s="1"/>
+      <c r="BY375" s="1"/>
+      <c r="CA375" s="1"/>
+      <c r="CC375" s="1"/>
+      <c r="CD375" s="1"/>
+      <c r="CF375" s="1"/>
+      <c r="CG375" s="1"/>
+      <c r="CH375" s="1"/>
+      <c r="CI375" s="1"/>
+      <c r="CJ375" s="1"/>
+      <c r="CK375" s="1"/>
+      <c r="CL375" s="1"/>
+      <c r="CM375" s="1"/>
+      <c r="CO375" s="1"/>
+      <c r="CP375" s="1"/>
+      <c r="CQ375" s="1"/>
+      <c r="CR375" s="1"/>
+      <c r="CS375" s="1"/>
+      <c r="CT375" s="1"/>
+      <c r="CU375" s="1"/>
+      <c r="CV375" s="1"/>
+      <c r="CW375" s="1"/>
+      <c r="CX375" s="1"/>
+      <c r="CY375" s="1"/>
+      <c r="CZ375" s="1"/>
+      <c r="DA375" s="1"/>
+      <c r="DB375" s="1"/>
+      <c r="DC375" s="1"/>
+      <c r="DD375" s="1"/>
+      <c r="DE375" s="1"/>
+      <c r="DF375" s="1"/>
+      <c r="DG375" s="1"/>
+      <c r="DI375" s="1"/>
+      <c r="DJ375" s="1"/>
+      <c r="DK375" s="1"/>
+      <c r="DL375" s="1"/>
+      <c r="DM375" s="1"/>
+      <c r="DN375" s="1"/>
+      <c r="DO375" s="1"/>
+      <c r="DP375" s="1"/>
+      <c r="DQ375" s="1"/>
+      <c r="DR375" s="1"/>
+      <c r="DS375" s="1"/>
+      <c r="DT375" s="1"/>
+      <c r="DU375" s="1"/>
+      <c r="DV375" s="1"/>
+      <c r="DW375" s="1"/>
+      <c r="DX375" s="1"/>
+      <c r="DY375" s="1"/>
+      <c r="DZ375" s="1"/>
+      <c r="EA375" s="1"/>
+      <c r="EB375" s="1"/>
+      <c r="ED375" s="1"/>
+      <c r="EE375" s="1"/>
+      <c r="EF375" s="1"/>
+      <c r="EG375" s="1"/>
+      <c r="EH375" s="1"/>
+      <c r="EI375" s="1"/>
+      <c r="EJ375" s="1"/>
+      <c r="EK375" s="1"/>
+      <c r="EL375" s="1"/>
+      <c r="EM375" s="1"/>
+      <c r="EN375" s="1"/>
+      <c r="EP375" s="1"/>
+      <c r="ER375" s="1"/>
+      <c r="ES375" s="1"/>
+      <c r="ET375" s="1"/>
+      <c r="EU375" s="1"/>
+      <c r="EV375" s="1"/>
+      <c r="EW375" s="1"/>
+      <c r="EX375" s="1"/>
+      <c r="EY375" s="1"/>
+      <c r="EZ375" s="1"/>
+      <c r="FA375" s="1"/>
+      <c r="FB375" s="1"/>
+      <c r="FC375" s="1"/>
+      <c r="FD375" s="1"/>
+      <c r="FF375" s="1"/>
+      <c r="FG375" s="1"/>
+      <c r="FH375" s="1"/>
+      <c r="FI375" s="1"/>
+      <c r="FJ375" s="1"/>
+      <c r="FK375" s="1"/>
+      <c r="FL375" s="1"/>
+      <c r="FM375" s="1"/>
+      <c r="FN375" s="1"/>
+      <c r="FO375" s="1"/>
+      <c r="FQ375" s="1"/>
+      <c r="FR375" s="1"/>
+      <c r="FS375" s="1"/>
+      <c r="FT375" s="1"/>
+      <c r="FU375" s="1"/>
+      <c r="FV375" s="1"/>
+      <c r="FW375" s="1"/>
+      <c r="FX375" s="1"/>
+      <c r="FY375" s="1"/>
+      <c r="FZ375" s="1"/>
+      <c r="GA375" s="1"/>
+      <c r="GC375" s="1"/>
+      <c r="GD375" s="1"/>
+      <c r="GE375" s="1"/>
+      <c r="GF375" s="1"/>
+      <c r="GG375" s="1"/>
+      <c r="GI375" s="1"/>
+      <c r="GJ375" s="1"/>
+      <c r="GK375" s="1"/>
+      <c r="GL375" s="1"/>
+      <c r="GM375" s="1"/>
+      <c r="GN375" s="1"/>
+      <c r="GO375" s="1"/>
+      <c r="GP375" s="1"/>
+      <c r="GQ375" s="1"/>
+      <c r="GR375" s="1"/>
+      <c r="GS375" s="1"/>
+      <c r="GT375" s="1"/>
+      <c r="GU375" s="1"/>
+      <c r="GV375" s="1"/>
+      <c r="GW375" s="1"/>
+      <c r="GX375" s="1"/>
+      <c r="GY375" s="1"/>
+      <c r="GZ375" s="1"/>
+      <c r="HA375" s="1"/>
+      <c r="HB375" s="1"/>
+      <c r="HD375" s="1"/>
+      <c r="HE375" s="1"/>
+      <c r="HF375" s="1"/>
+      <c r="HG375" s="1"/>
+      <c r="HI375" s="1"/>
+      <c r="HK375" s="1"/>
+      <c r="HL375" s="1"/>
+      <c r="HM375" s="1"/>
+      <c r="HN375" s="1"/>
+      <c r="HO375" s="1"/>
+      <c r="HP375" s="1"/>
+      <c r="HQ375" s="1"/>
+      <c r="HR375" s="1"/>
+      <c r="HS375" s="1"/>
+      <c r="HT375" s="1"/>
+      <c r="HU375" s="1"/>
+      <c r="HW375" s="1"/>
+      <c r="HX375" s="1"/>
+      <c r="HY375" s="1"/>
+      <c r="HZ375" s="1"/>
+      <c r="IA375" s="1"/>
+      <c r="IB375" s="1"/>
+      <c r="IC375" s="1"/>
+      <c r="ID375" s="1"/>
     </row>
-    <row r="376" spans="30:238" x14ac:dyDescent="0.3">
-      <c r="AD376" s="1"/>
-      <c r="AE376" s="1"/>
-      <c r="AF376" s="1"/>
-      <c r="AJ376" s="1"/>
-      <c r="AP376" s="1"/>
-      <c r="AQ376" s="1"/>
-      <c r="AT376" s="1"/>
-      <c r="AU376" s="1"/>
-      <c r="AX376" s="1"/>
-      <c r="AZ376" s="1"/>
-      <c r="BA376" s="1"/>
-      <c r="BB376" s="1"/>
-      <c r="BD376" s="1"/>
-      <c r="BF376" s="1"/>
-      <c r="BG376" s="1"/>
-      <c r="BH376" s="1"/>
-      <c r="BJ376" s="1"/>
-      <c r="BK376" s="1"/>
-      <c r="BM376" s="1"/>
-      <c r="BN376" s="1"/>
-      <c r="BO376" s="1"/>
-      <c r="BR376" s="1"/>
-      <c r="BT376" s="1"/>
-      <c r="BU376" s="1"/>
-      <c r="BV376" s="1"/>
-      <c r="BW376" s="1"/>
-      <c r="BX376" s="1"/>
-      <c r="BY376" s="1"/>
-      <c r="CA376" s="1"/>
-      <c r="CC376" s="1"/>
-      <c r="CD376" s="1"/>
-      <c r="CF376" s="1"/>
-      <c r="CG376" s="1"/>
-      <c r="CH376" s="1"/>
-      <c r="CI376" s="1"/>
-      <c r="CJ376" s="1"/>
-      <c r="CK376" s="1"/>
-      <c r="CL376" s="1"/>
-      <c r="CM376" s="1"/>
-      <c r="CO376" s="1"/>
-      <c r="CP376" s="1"/>
-      <c r="CQ376" s="1"/>
-      <c r="CR376" s="1"/>
-      <c r="CS376" s="1"/>
-      <c r="CT376" s="1"/>
-      <c r="CU376" s="1"/>
-      <c r="CV376" s="1"/>
-      <c r="CW376" s="1"/>
-      <c r="CX376" s="1"/>
-      <c r="CY376" s="1"/>
-      <c r="CZ376" s="1"/>
-      <c r="DA376" s="1"/>
-      <c r="DB376" s="1"/>
-      <c r="DC376" s="1"/>
-      <c r="DD376" s="1"/>
-      <c r="DE376" s="1"/>
-      <c r="DF376" s="1"/>
-      <c r="DG376" s="1"/>
-      <c r="DI376" s="1"/>
-      <c r="DJ376" s="1"/>
-      <c r="DK376" s="1"/>
-      <c r="DL376" s="1"/>
-      <c r="DM376" s="1"/>
-      <c r="DN376" s="1"/>
-      <c r="DO376" s="1"/>
-      <c r="DP376" s="1"/>
-      <c r="DQ376" s="1"/>
-      <c r="DR376" s="1"/>
-      <c r="DS376" s="1"/>
-      <c r="DT376" s="1"/>
-      <c r="DU376" s="1"/>
-      <c r="DV376" s="1"/>
-      <c r="DW376" s="1"/>
-      <c r="DX376" s="1"/>
-      <c r="DY376" s="1"/>
-      <c r="DZ376" s="1"/>
-      <c r="EA376" s="1"/>
-      <c r="EB376" s="1"/>
-      <c r="ED376" s="1"/>
-      <c r="EE376" s="1"/>
-      <c r="EF376" s="1"/>
-      <c r="EG376" s="1"/>
-      <c r="EH376" s="1"/>
-      <c r="EI376" s="1"/>
-      <c r="EJ376" s="1"/>
-      <c r="EK376" s="1"/>
-      <c r="EL376" s="1"/>
-      <c r="EM376" s="1"/>
-      <c r="EN376" s="1"/>
-      <c r="EP376" s="1"/>
-      <c r="ER376" s="1"/>
-      <c r="ES376" s="1"/>
-      <c r="ET376" s="1"/>
-      <c r="EU376" s="1"/>
-      <c r="EV376" s="1"/>
-      <c r="EW376" s="1"/>
-      <c r="EX376" s="1"/>
-      <c r="EY376" s="1"/>
-      <c r="EZ376" s="1"/>
-      <c r="FA376" s="1"/>
-      <c r="FB376" s="1"/>
-      <c r="FC376" s="1"/>
-      <c r="FD376" s="1"/>
-      <c r="FF376" s="1"/>
-      <c r="FG376" s="1"/>
-      <c r="FH376" s="1"/>
-      <c r="FI376" s="1"/>
-      <c r="FJ376" s="1"/>
-      <c r="FK376" s="1"/>
-      <c r="FL376" s="1"/>
-      <c r="FM376" s="1"/>
-      <c r="FN376" s="1"/>
-      <c r="FO376" s="1"/>
-      <c r="FQ376" s="1"/>
-      <c r="FR376" s="1"/>
-      <c r="FS376" s="1"/>
-      <c r="FT376" s="1"/>
-      <c r="FU376" s="1"/>
-      <c r="FV376" s="1"/>
-      <c r="FW376" s="1"/>
-      <c r="FX376" s="1"/>
-      <c r="FY376" s="1"/>
-      <c r="FZ376" s="1"/>
-      <c r="GA376" s="1"/>
-      <c r="GC376" s="1"/>
-      <c r="GD376" s="1"/>
-      <c r="GE376" s="1"/>
-      <c r="GF376" s="1"/>
-      <c r="GG376" s="1"/>
-      <c r="GI376" s="1"/>
-      <c r="GJ376" s="1"/>
-      <c r="GK376" s="1"/>
-      <c r="GL376" s="1"/>
-      <c r="GM376" s="1"/>
-      <c r="GN376" s="1"/>
-      <c r="GO376" s="1"/>
-      <c r="GP376" s="1"/>
-      <c r="GQ376" s="1"/>
-      <c r="GR376" s="1"/>
-      <c r="GS376" s="1"/>
-      <c r="GT376" s="1"/>
-      <c r="GU376" s="1"/>
-      <c r="GV376" s="1"/>
-      <c r="GW376" s="1"/>
-      <c r="GX376" s="1"/>
-      <c r="GY376" s="1"/>
-      <c r="GZ376" s="1"/>
-      <c r="HA376" s="1"/>
-      <c r="HB376" s="1"/>
-      <c r="HD376" s="1"/>
-      <c r="HE376" s="1"/>
-      <c r="HF376" s="1"/>
-      <c r="HG376" s="1"/>
-      <c r="HI376" s="1"/>
-      <c r="HK376" s="1"/>
-      <c r="HL376" s="1"/>
-      <c r="HM376" s="1"/>
-      <c r="HN376" s="1"/>
-      <c r="HO376" s="1"/>
-      <c r="HP376" s="1"/>
-      <c r="HQ376" s="1"/>
-      <c r="HR376" s="1"/>
-      <c r="HS376" s="1"/>
-      <c r="HT376" s="1"/>
-      <c r="HU376" s="1"/>
-      <c r="HW376" s="1"/>
-      <c r="HX376" s="1"/>
-      <c r="HY376" s="1"/>
-      <c r="HZ376" s="1"/>
-      <c r="IA376" s="1"/>
-      <c r="IB376" s="1"/>
-      <c r="IC376" s="1"/>
-      <c r="ID376" s="1"/>
+    <row r="409" spans="112:242" x14ac:dyDescent="0.3">
+      <c r="DH409" s="1"/>
+      <c r="EO409" s="1"/>
+      <c r="ET409" s="1"/>
+      <c r="FE409" s="1"/>
+      <c r="FP409" s="1"/>
+      <c r="FV409" s="1"/>
+      <c r="GB409" s="1"/>
+      <c r="GD409" s="1"/>
+      <c r="GF409" s="1"/>
+      <c r="GI409" s="1"/>
+      <c r="GK409" s="1"/>
+      <c r="GM409" s="1"/>
+      <c r="GR409" s="1"/>
+      <c r="GV409" s="1"/>
+      <c r="GW409" s="1"/>
+      <c r="HC409" s="1"/>
+      <c r="HF409" s="1"/>
+      <c r="HH409" s="1"/>
+      <c r="HI409" s="1"/>
+      <c r="HJ409" s="1"/>
+      <c r="HQ409" s="1"/>
+      <c r="HV409" s="1"/>
+      <c r="HW409" s="1"/>
+      <c r="IE409" s="1"/>
+      <c r="IF409" s="1"/>
+      <c r="IG409" s="1"/>
+      <c r="IH409" s="1"/>
     </row>
     <row r="410" spans="112:242" x14ac:dyDescent="0.3">
       <c r="DH410" s="1"/>
-      <c r="EO410" s="1"/>
-      <c r="ET410" s="1"/>
-      <c r="FE410" s="1"/>
-      <c r="FP410" s="1"/>
-      <c r="FV410" s="1"/>
-      <c r="GB410" s="1"/>
-      <c r="GD410" s="1"/>
-      <c r="GF410" s="1"/>
-      <c r="GI410" s="1"/>
-      <c r="GK410" s="1"/>
-      <c r="GM410" s="1"/>
-      <c r="GR410" s="1"/>
-      <c r="GV410" s="1"/>
-      <c r="GW410" s="1"/>
       <c r="HC410" s="1"/>
-      <c r="HF410" s="1"/>
-      <c r="HH410" s="1"/>
-      <c r="HI410" s="1"/>
-      <c r="HJ410" s="1"/>
-      <c r="HQ410" s="1"/>
-      <c r="HV410" s="1"/>
-      <c r="HW410" s="1"/>
-      <c r="IE410" s="1"/>
-      <c r="IF410" s="1"/>
-      <c r="IG410" s="1"/>
-      <c r="IH410" s="1"/>
     </row>
-    <row r="411" spans="112:242" x14ac:dyDescent="0.3">
-      <c r="DH411" s="1"/>
-      <c r="HC411" s="1"/>
+    <row r="426" spans="33:233" x14ac:dyDescent="0.3">
+      <c r="AG426" s="1"/>
+      <c r="CJ426" s="1"/>
+      <c r="CO426" s="1"/>
+      <c r="DW426" s="1"/>
+      <c r="HR426" s="1"/>
+      <c r="HY426" s="1"/>
     </row>
-    <row r="427" spans="33:233" x14ac:dyDescent="0.3">
-      <c r="AG427" s="1"/>
-      <c r="CJ427" s="1"/>
-      <c r="CO427" s="1"/>
-      <c r="DW427" s="1"/>
-      <c r="HR427" s="1"/>
-      <c r="HY427" s="1"/>
+    <row r="455" spans="226:226" x14ac:dyDescent="0.3">
+      <c r="HR455" s="1"/>
     </row>
-    <row r="456" spans="226:226" x14ac:dyDescent="0.3">
-      <c r="HR456" s="1"/>
+    <row r="459" spans="226:226" x14ac:dyDescent="0.3">
+      <c r="HR459" s="1"/>
     </row>
-    <row r="460" spans="226:226" x14ac:dyDescent="0.3">
-      <c r="HR460" s="1"/>
+    <row r="467" spans="22:242" x14ac:dyDescent="0.3">
+      <c r="V467" s="1"/>
+      <c r="W467" s="1"/>
+      <c r="X467" s="1"/>
+      <c r="Y467" s="1"/>
+      <c r="Z467" s="1"/>
+      <c r="AB467" s="1"/>
+      <c r="AD467" s="1"/>
+      <c r="AE467" s="1"/>
+      <c r="AF467" s="1"/>
+      <c r="AG467" s="1"/>
+      <c r="AH467" s="1"/>
+      <c r="AI467" s="1"/>
+      <c r="AJ467" s="1"/>
+      <c r="AK467" s="1"/>
+      <c r="AL467" s="1"/>
+      <c r="AM467" s="1"/>
+      <c r="AN467" s="1"/>
+      <c r="AO467" s="1"/>
+      <c r="AP467" s="1"/>
+      <c r="AQ467" s="1"/>
+      <c r="AR467" s="1"/>
+      <c r="AS467" s="1"/>
+      <c r="AT467" s="1"/>
+      <c r="AU467" s="1"/>
+      <c r="AV467" s="1"/>
+      <c r="AW467" s="1"/>
+      <c r="AX467" s="1"/>
+      <c r="AY467" s="1"/>
+      <c r="AZ467" s="1"/>
+      <c r="BA467" s="1"/>
+      <c r="BB467" s="1"/>
+      <c r="BC467" s="1"/>
+      <c r="BD467" s="1"/>
+      <c r="BE467" s="1"/>
+      <c r="BF467" s="1"/>
+      <c r="BG467" s="1"/>
+      <c r="BH467" s="1"/>
+      <c r="BI467" s="1"/>
+      <c r="BJ467" s="1"/>
+      <c r="BK467" s="1"/>
+      <c r="BL467" s="1"/>
+      <c r="BM467" s="1"/>
+      <c r="BN467" s="1"/>
+      <c r="BO467" s="1"/>
+      <c r="BP467" s="1"/>
+      <c r="BQ467" s="1"/>
+      <c r="BR467" s="1"/>
+      <c r="BS467" s="1"/>
+      <c r="BT467" s="1"/>
+      <c r="BU467" s="1"/>
+      <c r="BV467" s="1"/>
+      <c r="BW467" s="1"/>
+      <c r="BX467" s="1"/>
+      <c r="BY467" s="1"/>
+      <c r="BZ467" s="1"/>
+      <c r="CA467" s="1"/>
+      <c r="CB467" s="1"/>
+      <c r="CC467" s="1"/>
+      <c r="CD467" s="1"/>
+      <c r="CE467" s="1"/>
+      <c r="CF467" s="1"/>
+      <c r="CG467" s="1"/>
+      <c r="CH467" s="1"/>
+      <c r="CI467" s="1"/>
+      <c r="CJ467" s="1"/>
+      <c r="CK467" s="1"/>
+      <c r="CL467" s="1"/>
+      <c r="CM467" s="1"/>
+      <c r="CN467" s="1"/>
+      <c r="CO467" s="1"/>
+      <c r="CP467" s="1"/>
+      <c r="CQ467" s="1"/>
+      <c r="CR467" s="1"/>
+      <c r="CS467" s="1"/>
+      <c r="CT467" s="1"/>
+      <c r="CU467" s="1"/>
+      <c r="CV467" s="1"/>
+      <c r="CW467" s="1"/>
+      <c r="CX467" s="1"/>
+      <c r="CY467" s="1"/>
+      <c r="CZ467" s="1"/>
+      <c r="DA467" s="1"/>
+      <c r="DB467" s="1"/>
+      <c r="DC467" s="1"/>
+      <c r="DD467" s="1"/>
+      <c r="DE467" s="1"/>
+      <c r="DF467" s="1"/>
+      <c r="DG467" s="1"/>
+      <c r="DH467" s="1"/>
+      <c r="DI467" s="1"/>
+      <c r="DJ467" s="1"/>
+      <c r="DK467" s="1"/>
+      <c r="DL467" s="1"/>
+      <c r="DM467" s="1"/>
+      <c r="DN467" s="1"/>
+      <c r="DO467" s="1"/>
+      <c r="DP467" s="1"/>
+      <c r="DQ467" s="1"/>
+      <c r="DR467" s="1"/>
+      <c r="DS467" s="1"/>
+      <c r="DT467" s="1"/>
+      <c r="DU467" s="1"/>
+      <c r="DV467" s="1"/>
+      <c r="DW467" s="1"/>
+      <c r="DX467" s="1"/>
+      <c r="DY467" s="1"/>
+      <c r="DZ467" s="1"/>
+      <c r="EA467" s="1"/>
+      <c r="EB467" s="1"/>
+      <c r="EC467" s="1"/>
+      <c r="ED467" s="1"/>
+      <c r="EE467" s="1"/>
+      <c r="EF467" s="1"/>
+      <c r="EG467" s="1"/>
+      <c r="EH467" s="1"/>
+      <c r="EI467" s="1"/>
+      <c r="EJ467" s="1"/>
+      <c r="EK467" s="1"/>
+      <c r="EL467" s="1"/>
+      <c r="EM467" s="1"/>
+      <c r="EN467" s="1"/>
+      <c r="EO467" s="1"/>
+      <c r="EP467" s="1"/>
+      <c r="EQ467" s="1"/>
+      <c r="ER467" s="1"/>
+      <c r="ES467" s="1"/>
+      <c r="ET467" s="1"/>
+      <c r="EU467" s="1"/>
+      <c r="EV467" s="1"/>
+      <c r="EW467" s="1"/>
+      <c r="EX467" s="1"/>
+      <c r="EY467" s="1"/>
+      <c r="EZ467" s="1"/>
+      <c r="FA467" s="1"/>
+      <c r="FB467" s="1"/>
+      <c r="FC467" s="1"/>
+      <c r="FD467" s="1"/>
+      <c r="FE467" s="1"/>
+      <c r="FF467" s="1"/>
+      <c r="FG467" s="1"/>
+      <c r="FH467" s="1"/>
+      <c r="FI467" s="1"/>
+      <c r="FJ467" s="1"/>
+      <c r="FK467" s="1"/>
+      <c r="FL467" s="1"/>
+      <c r="FM467" s="1"/>
+      <c r="FN467" s="1"/>
+      <c r="FO467" s="1"/>
+      <c r="FP467" s="1"/>
+      <c r="FQ467" s="1"/>
+      <c r="FR467" s="1"/>
+      <c r="FS467" s="1"/>
+      <c r="FT467" s="1"/>
+      <c r="FU467" s="1"/>
+      <c r="FV467" s="1"/>
+      <c r="FW467" s="1"/>
+      <c r="FX467" s="1"/>
+      <c r="FY467" s="1"/>
+      <c r="FZ467" s="1"/>
+      <c r="GA467" s="1"/>
+      <c r="GC467" s="1"/>
+      <c r="GD467" s="1"/>
+      <c r="GE467" s="1"/>
+      <c r="GF467" s="1"/>
+      <c r="GG467" s="1"/>
+      <c r="GH467" s="1"/>
+      <c r="GI467" s="1"/>
+      <c r="GJ467" s="1"/>
+      <c r="GK467" s="1"/>
+      <c r="GL467" s="1"/>
+      <c r="GM467" s="1"/>
+      <c r="GN467" s="1"/>
+      <c r="GO467" s="1"/>
+      <c r="GP467" s="1"/>
+      <c r="GQ467" s="1"/>
+      <c r="GR467" s="1"/>
+      <c r="GS467" s="1"/>
+      <c r="GT467" s="1"/>
+      <c r="GU467" s="1"/>
+      <c r="GV467" s="1"/>
+      <c r="GW467" s="1"/>
+      <c r="GX467" s="1"/>
+      <c r="GY467" s="1"/>
+      <c r="GZ467" s="1"/>
+      <c r="HA467" s="1"/>
+      <c r="HB467" s="1"/>
+      <c r="HC467" s="1"/>
+      <c r="HD467" s="1"/>
+      <c r="HE467" s="1"/>
+      <c r="HF467" s="1"/>
+      <c r="HG467" s="1"/>
+      <c r="HH467" s="1"/>
+      <c r="HI467" s="1"/>
+      <c r="HK467" s="1"/>
+      <c r="HL467" s="1"/>
+      <c r="HM467" s="1"/>
+      <c r="HN467" s="1"/>
+      <c r="HO467" s="1"/>
+      <c r="HP467" s="1"/>
+      <c r="HQ467" s="1"/>
+      <c r="HR467" s="1"/>
+      <c r="HS467" s="1"/>
+      <c r="HT467" s="1"/>
+      <c r="HU467" s="1"/>
+      <c r="HV467" s="1"/>
+      <c r="HW467" s="1"/>
+      <c r="HX467" s="1"/>
+      <c r="HY467" s="1"/>
+      <c r="HZ467" s="1"/>
+      <c r="IA467" s="1"/>
+      <c r="IB467" s="1"/>
+      <c r="IC467" s="1"/>
+      <c r="ID467" s="1"/>
+      <c r="IE467" s="1"/>
+      <c r="IF467" s="1"/>
+      <c r="IG467" s="1"/>
+      <c r="IH467" s="1"/>
     </row>
-    <row r="468" spans="22:242" x14ac:dyDescent="0.3">
-      <c r="V468" s="1"/>
-      <c r="W468" s="1"/>
-      <c r="X468" s="1"/>
-      <c r="Y468" s="1"/>
-      <c r="Z468" s="1"/>
-      <c r="AB468" s="1"/>
-      <c r="AD468" s="1"/>
-      <c r="AE468" s="1"/>
-      <c r="AF468" s="1"/>
-      <c r="AG468" s="1"/>
-      <c r="AH468" s="1"/>
-      <c r="AI468" s="1"/>
-      <c r="AJ468" s="1"/>
-      <c r="AK468" s="1"/>
-      <c r="AL468" s="1"/>
-      <c r="AM468" s="1"/>
-      <c r="AN468" s="1"/>
-      <c r="AO468" s="1"/>
-      <c r="AP468" s="1"/>
-      <c r="AQ468" s="1"/>
-      <c r="AR468" s="1"/>
-      <c r="AS468" s="1"/>
-      <c r="AT468" s="1"/>
-      <c r="AU468" s="1"/>
-      <c r="AV468" s="1"/>
-      <c r="AW468" s="1"/>
-      <c r="AX468" s="1"/>
-      <c r="AY468" s="1"/>
-      <c r="AZ468" s="1"/>
-      <c r="BA468" s="1"/>
-      <c r="BB468" s="1"/>
-      <c r="BC468" s="1"/>
-      <c r="BD468" s="1"/>
-      <c r="BE468" s="1"/>
-      <c r="BF468" s="1"/>
-      <c r="BG468" s="1"/>
-      <c r="BH468" s="1"/>
-      <c r="BI468" s="1"/>
-      <c r="BJ468" s="1"/>
-      <c r="BK468" s="1"/>
-      <c r="BL468" s="1"/>
-      <c r="BM468" s="1"/>
-      <c r="BN468" s="1"/>
-      <c r="BO468" s="1"/>
-      <c r="BP468" s="1"/>
-      <c r="BQ468" s="1"/>
-      <c r="BR468" s="1"/>
-      <c r="BS468" s="1"/>
-      <c r="BT468" s="1"/>
-      <c r="BU468" s="1"/>
-      <c r="BV468" s="1"/>
-      <c r="BW468" s="1"/>
-      <c r="BX468" s="1"/>
-      <c r="BY468" s="1"/>
-      <c r="BZ468" s="1"/>
-      <c r="CA468" s="1"/>
-      <c r="CB468" s="1"/>
-      <c r="CC468" s="1"/>
-      <c r="CD468" s="1"/>
-      <c r="CE468" s="1"/>
-      <c r="CF468" s="1"/>
-      <c r="CG468" s="1"/>
-      <c r="CH468" s="1"/>
-      <c r="CI468" s="1"/>
-      <c r="CJ468" s="1"/>
-      <c r="CK468" s="1"/>
-      <c r="CL468" s="1"/>
-      <c r="CM468" s="1"/>
-      <c r="CN468" s="1"/>
-      <c r="CO468" s="1"/>
-      <c r="CP468" s="1"/>
-      <c r="CQ468" s="1"/>
-      <c r="CR468" s="1"/>
-      <c r="CS468" s="1"/>
-      <c r="CT468" s="1"/>
-      <c r="CU468" s="1"/>
-      <c r="CV468" s="1"/>
-      <c r="CW468" s="1"/>
-      <c r="CX468" s="1"/>
-      <c r="CY468" s="1"/>
-      <c r="CZ468" s="1"/>
-      <c r="DA468" s="1"/>
-      <c r="DB468" s="1"/>
-      <c r="DC468" s="1"/>
-      <c r="DD468" s="1"/>
-      <c r="DE468" s="1"/>
-      <c r="DF468" s="1"/>
-      <c r="DG468" s="1"/>
-      <c r="DH468" s="1"/>
-      <c r="DI468" s="1"/>
-      <c r="DJ468" s="1"/>
-      <c r="DK468" s="1"/>
-      <c r="DL468" s="1"/>
-      <c r="DM468" s="1"/>
-      <c r="DN468" s="1"/>
-      <c r="DO468" s="1"/>
-      <c r="DP468" s="1"/>
-      <c r="DQ468" s="1"/>
-      <c r="DR468" s="1"/>
-      <c r="DS468" s="1"/>
-      <c r="DT468" s="1"/>
-      <c r="DU468" s="1"/>
-      <c r="DV468" s="1"/>
-      <c r="DW468" s="1"/>
-      <c r="DX468" s="1"/>
-      <c r="DY468" s="1"/>
-      <c r="DZ468" s="1"/>
-      <c r="EA468" s="1"/>
-      <c r="EB468" s="1"/>
-      <c r="EC468" s="1"/>
-      <c r="ED468" s="1"/>
-      <c r="EE468" s="1"/>
-      <c r="EF468" s="1"/>
-      <c r="EG468" s="1"/>
-      <c r="EH468" s="1"/>
-      <c r="EI468" s="1"/>
-      <c r="EJ468" s="1"/>
-      <c r="EK468" s="1"/>
-      <c r="EL468" s="1"/>
-      <c r="EM468" s="1"/>
-      <c r="EN468" s="1"/>
-      <c r="EO468" s="1"/>
-      <c r="EP468" s="1"/>
-      <c r="EQ468" s="1"/>
-      <c r="ER468" s="1"/>
-      <c r="ES468" s="1"/>
-      <c r="ET468" s="1"/>
-      <c r="EU468" s="1"/>
-      <c r="EV468" s="1"/>
-      <c r="EW468" s="1"/>
-      <c r="EX468" s="1"/>
-      <c r="EY468" s="1"/>
-      <c r="EZ468" s="1"/>
-      <c r="FA468" s="1"/>
-      <c r="FB468" s="1"/>
-      <c r="FC468" s="1"/>
-      <c r="FD468" s="1"/>
-      <c r="FE468" s="1"/>
-      <c r="FF468" s="1"/>
-      <c r="FG468" s="1"/>
-      <c r="FH468" s="1"/>
-      <c r="FI468" s="1"/>
-      <c r="FJ468" s="1"/>
-      <c r="FK468" s="1"/>
-      <c r="FL468" s="1"/>
-      <c r="FM468" s="1"/>
-      <c r="FN468" s="1"/>
-      <c r="FO468" s="1"/>
-      <c r="FP468" s="1"/>
-      <c r="FQ468" s="1"/>
-      <c r="FR468" s="1"/>
-      <c r="FS468" s="1"/>
-      <c r="FT468" s="1"/>
-      <c r="FU468" s="1"/>
-      <c r="FV468" s="1"/>
-      <c r="FW468" s="1"/>
-      <c r="FX468" s="1"/>
-      <c r="FY468" s="1"/>
-      <c r="FZ468" s="1"/>
-      <c r="GA468" s="1"/>
-      <c r="GC468" s="1"/>
-      <c r="GD468" s="1"/>
-      <c r="GE468" s="1"/>
-      <c r="GF468" s="1"/>
-      <c r="GG468" s="1"/>
-      <c r="GH468" s="1"/>
-      <c r="GI468" s="1"/>
-      <c r="GJ468" s="1"/>
-      <c r="GK468" s="1"/>
-      <c r="GL468" s="1"/>
-      <c r="GM468" s="1"/>
-      <c r="GN468" s="1"/>
-      <c r="GO468" s="1"/>
-      <c r="GP468" s="1"/>
-      <c r="GQ468" s="1"/>
-      <c r="GR468" s="1"/>
-      <c r="GS468" s="1"/>
-      <c r="GT468" s="1"/>
-      <c r="GU468" s="1"/>
-      <c r="GV468" s="1"/>
-      <c r="GW468" s="1"/>
-      <c r="GX468" s="1"/>
-      <c r="GY468" s="1"/>
-      <c r="GZ468" s="1"/>
-      <c r="HA468" s="1"/>
-      <c r="HB468" s="1"/>
-      <c r="HC468" s="1"/>
-      <c r="HD468" s="1"/>
-      <c r="HE468" s="1"/>
-      <c r="HF468" s="1"/>
-      <c r="HG468" s="1"/>
-      <c r="HH468" s="1"/>
-      <c r="HI468" s="1"/>
-      <c r="HK468" s="1"/>
-      <c r="HL468" s="1"/>
-      <c r="HM468" s="1"/>
-      <c r="HN468" s="1"/>
-      <c r="HO468" s="1"/>
-      <c r="HP468" s="1"/>
-      <c r="HQ468" s="1"/>
-      <c r="HR468" s="1"/>
-      <c r="HS468" s="1"/>
-      <c r="HT468" s="1"/>
-      <c r="HU468" s="1"/>
-      <c r="HV468" s="1"/>
-      <c r="HW468" s="1"/>
-      <c r="HX468" s="1"/>
-      <c r="HY468" s="1"/>
-      <c r="HZ468" s="1"/>
-      <c r="IA468" s="1"/>
-      <c r="IB468" s="1"/>
-      <c r="IC468" s="1"/>
-      <c r="ID468" s="1"/>
-      <c r="IE468" s="1"/>
-      <c r="IF468" s="1"/>
-      <c r="IG468" s="1"/>
-      <c r="IH468" s="1"/>
+    <row r="493" spans="192:212" x14ac:dyDescent="0.3">
+      <c r="GJ493" s="1"/>
+      <c r="GN493" s="1"/>
+      <c r="GW493" s="1"/>
+      <c r="HD493" s="1"/>
     </row>
-    <row r="494" spans="192:212" x14ac:dyDescent="0.3">
-      <c r="GJ494" s="1"/>
-      <c r="GN494" s="1"/>
-      <c r="GW494" s="1"/>
-      <c r="HD494" s="1"/>
+    <row r="506" spans="30:30" x14ac:dyDescent="0.3">
+      <c r="AD506" s="1"/>
     </row>
-    <row r="507" spans="30:30" x14ac:dyDescent="0.3">
-      <c r="AD507" s="1"/>
+    <row r="609" spans="45:59" x14ac:dyDescent="0.3">
+      <c r="AS609" s="1"/>
+      <c r="AT609" s="1"/>
+      <c r="BG609" s="1"/>
     </row>
-    <row r="610" spans="45:59" x14ac:dyDescent="0.3">
-      <c r="AS610" s="1"/>
-      <c r="AT610" s="1"/>
-      <c r="BG610" s="1"/>
+    <row r="644" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA644" s="1"/>
     </row>
     <row r="645" spans="27:27" x14ac:dyDescent="0.3">
       <c r="AA645" s="1"/>
     </row>
-    <row r="646" spans="27:27" x14ac:dyDescent="0.3">
-      <c r="AA646" s="1"/>
+    <row r="736" spans="147:152" x14ac:dyDescent="0.3">
+      <c r="EQ736" s="1"/>
+      <c r="EV736" s="1"/>
     </row>
-    <row r="737" spans="147:152" x14ac:dyDescent="0.3">
-      <c r="EQ737" s="1"/>
-      <c r="EV737" s="1"/>
+    <row r="1073" spans="218:218" x14ac:dyDescent="0.3">
+      <c r="HJ1073" s="1"/>
     </row>
     <row r="1074" spans="218:218" x14ac:dyDescent="0.3">
       <c r="HJ1074" s="1"/>
     </row>
-    <row r="1075" spans="218:218" x14ac:dyDescent="0.3">
-      <c r="HJ1075" s="1"/>
+    <row r="1251" spans="39:242" x14ac:dyDescent="0.3">
+      <c r="AM1251" s="1"/>
+      <c r="AR1251" s="1"/>
+      <c r="AU1251" s="1"/>
+      <c r="AV1251" s="1"/>
+      <c r="HY1251" s="1"/>
+      <c r="IA1251" s="1"/>
+      <c r="IF1251" s="1"/>
+      <c r="IH1251" s="1"/>
     </row>
     <row r="1252" spans="39:242" x14ac:dyDescent="0.3">
-      <c r="AM1252" s="1"/>
-      <c r="AR1252" s="1"/>
-      <c r="AU1252" s="1"/>
-      <c r="AV1252" s="1"/>
-      <c r="HY1252" s="1"/>
-      <c r="IA1252" s="1"/>
-      <c r="IF1252" s="1"/>
-      <c r="IH1252" s="1"/>
+      <c r="CK1252" s="1"/>
+      <c r="CN1252" s="1"/>
+      <c r="CP1252" s="1"/>
+      <c r="CQ1252" s="1"/>
+      <c r="CR1252" s="1"/>
+      <c r="CS1252" s="1"/>
+      <c r="CT1252" s="1"/>
+      <c r="CU1252" s="1"/>
+      <c r="CV1252" s="1"/>
+      <c r="CW1252" s="1"/>
+      <c r="CY1252" s="1"/>
+      <c r="CZ1252" s="1"/>
+      <c r="DA1252" s="1"/>
+      <c r="DC1252" s="1"/>
+      <c r="DD1252" s="1"/>
+      <c r="DE1252" s="1"/>
+      <c r="DF1252" s="1"/>
+      <c r="DG1252" s="1"/>
+      <c r="DH1252" s="1"/>
+      <c r="DI1252" s="1"/>
+      <c r="DK1252" s="1"/>
+      <c r="DL1252" s="1"/>
+      <c r="DN1252" s="1"/>
+      <c r="DO1252" s="1"/>
+      <c r="DS1252" s="1"/>
+      <c r="EC1252" s="1"/>
     </row>
-    <row r="1253" spans="39:242" x14ac:dyDescent="0.3">
-      <c r="CK1253" s="1"/>
-      <c r="CN1253" s="1"/>
-      <c r="CP1253" s="1"/>
-      <c r="CQ1253" s="1"/>
-      <c r="CR1253" s="1"/>
-      <c r="CS1253" s="1"/>
-      <c r="CT1253" s="1"/>
-      <c r="CU1253" s="1"/>
-      <c r="CV1253" s="1"/>
-      <c r="CW1253" s="1"/>
-      <c r="CY1253" s="1"/>
-      <c r="CZ1253" s="1"/>
-      <c r="DA1253" s="1"/>
-      <c r="DC1253" s="1"/>
-      <c r="DD1253" s="1"/>
-      <c r="DE1253" s="1"/>
-      <c r="DF1253" s="1"/>
-      <c r="DG1253" s="1"/>
-      <c r="DH1253" s="1"/>
-      <c r="DI1253" s="1"/>
-      <c r="DK1253" s="1"/>
-      <c r="DL1253" s="1"/>
-      <c r="DN1253" s="1"/>
-      <c r="DO1253" s="1"/>
-      <c r="DS1253" s="1"/>
-      <c r="EC1253" s="1"/>
+    <row r="1255" spans="39:242" x14ac:dyDescent="0.3">
+      <c r="CC1255" s="1"/>
+      <c r="CG1255" s="1"/>
+      <c r="CI1255" s="1"/>
+      <c r="CK1255" s="1"/>
+      <c r="CN1255" s="1"/>
+      <c r="CT1255" s="1"/>
     </row>
-    <row r="1256" spans="39:242" x14ac:dyDescent="0.3">
-      <c r="CC1256" s="1"/>
-      <c r="CG1256" s="1"/>
-      <c r="CI1256" s="1"/>
-      <c r="CK1256" s="1"/>
-      <c r="CN1256" s="1"/>
-      <c r="CT1256" s="1"/>
+    <row r="1296" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA1296" s="1"/>
     </row>
-    <row r="1297" spans="27:27" x14ac:dyDescent="0.3">
-      <c r="AA1297" s="1"/>
+    <row r="1492" spans="129:129" x14ac:dyDescent="0.3">
+      <c r="DY1492" s="1"/>
     </row>
-    <row r="1493" spans="129:129" x14ac:dyDescent="0.3">
-      <c r="DY1493" s="1"/>
+    <row r="1556" spans="27:226" x14ac:dyDescent="0.3">
+      <c r="AA1556" s="1"/>
+      <c r="AC1556" s="1"/>
+      <c r="AJ1556" s="1"/>
+      <c r="BG1556" s="1"/>
+      <c r="BK1556" s="1"/>
+      <c r="EB1556" s="1"/>
+      <c r="FG1556" s="1"/>
+      <c r="GE1556" s="1"/>
+      <c r="HR1556" s="1"/>
     </row>
-    <row r="1557" spans="27:226" x14ac:dyDescent="0.3">
-      <c r="AA1557" s="1"/>
-      <c r="AC1557" s="1"/>
-      <c r="AJ1557" s="1"/>
-      <c r="BG1557" s="1"/>
-      <c r="BK1557" s="1"/>
-      <c r="EB1557" s="1"/>
-      <c r="FG1557" s="1"/>
-      <c r="GE1557" s="1"/>
-      <c r="HR1557" s="1"/>
+    <row r="1658" spans="27:187" x14ac:dyDescent="0.3">
+      <c r="AA1658" s="1"/>
+      <c r="AC1658" s="1"/>
+      <c r="BG1658" s="1"/>
+      <c r="GE1658" s="1"/>
     </row>
-    <row r="1659" spans="27:187" x14ac:dyDescent="0.3">
-      <c r="AA1659" s="1"/>
-      <c r="AC1659" s="1"/>
-      <c r="BG1659" s="1"/>
-      <c r="GE1659" s="1"/>
+    <row r="1673" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA1673" s="1"/>
     </row>
-    <row r="1674" spans="27:27" x14ac:dyDescent="0.3">
-      <c r="AA1674" s="1"/>
+    <row r="1765" spans="31:50" x14ac:dyDescent="0.3">
+      <c r="AE1765" s="1"/>
+      <c r="AX1765" s="1"/>
     </row>
-    <row r="1766" spans="31:50" x14ac:dyDescent="0.3">
-      <c r="AE1766" s="1"/>
-      <c r="AX1766" s="1"/>
+    <row r="1864" spans="149:149" x14ac:dyDescent="0.3">
+      <c r="ES1864" s="1"/>
     </row>
-    <row r="1865" spans="149:149" x14ac:dyDescent="0.3">
-      <c r="ES1865" s="1"/>
+    <row r="1878" spans="30:30" x14ac:dyDescent="0.3">
+      <c r="AD1878" s="1"/>
     </row>
-    <row r="1879" spans="30:30" x14ac:dyDescent="0.3">
-      <c r="AD1879" s="1"/>
+    <row r="1994" spans="22:32" x14ac:dyDescent="0.3">
+      <c r="V1994" s="1"/>
+      <c r="W1994" s="1"/>
+      <c r="X1994" s="1"/>
+      <c r="Y1994" s="1"/>
+      <c r="AB1994" s="1"/>
+      <c r="AE1994" s="1"/>
+      <c r="AF1994" s="1"/>
     </row>
-    <row r="1995" spans="22:32" x14ac:dyDescent="0.3">
-      <c r="V1995" s="1"/>
-      <c r="W1995" s="1"/>
-      <c r="X1995" s="1"/>
-      <c r="Y1995" s="1"/>
-      <c r="AB1995" s="1"/>
-      <c r="AE1995" s="1"/>
-      <c r="AF1995" s="1"/>
+    <row r="2307" spans="129:129" x14ac:dyDescent="0.3">
+      <c r="DY2307" s="1"/>
     </row>
-    <row r="2308" spans="129:129" x14ac:dyDescent="0.3">
-      <c r="DY2308" s="1"/>
+    <row r="2386" spans="22:225" x14ac:dyDescent="0.3">
+      <c r="V2386" s="1"/>
+      <c r="Z2386" s="1"/>
+      <c r="AA2386" s="1"/>
+      <c r="AI2386" s="1"/>
+      <c r="AV2386" s="1"/>
+      <c r="AW2386" s="1"/>
+      <c r="BE2386" s="1"/>
+      <c r="BF2386" s="1"/>
+      <c r="BI2386" s="1"/>
+      <c r="BP2386" s="1"/>
+      <c r="BQ2386" s="1"/>
+      <c r="BV2386" s="1"/>
+      <c r="CF2386" s="1"/>
+      <c r="CI2386" s="1"/>
+      <c r="CL2386" s="1"/>
+      <c r="CS2386" s="1"/>
+      <c r="CV2386" s="1"/>
+      <c r="DI2386" s="1"/>
+      <c r="DT2386" s="1"/>
+      <c r="DY2386" s="1"/>
+      <c r="EI2386" s="1"/>
+      <c r="EQ2386" s="1"/>
+      <c r="ES2386" s="1"/>
+      <c r="EV2386" s="1"/>
+      <c r="FE2386" s="1"/>
+      <c r="FF2386" s="1"/>
+      <c r="FJ2386" s="1"/>
+      <c r="FK2386" s="1"/>
+      <c r="FP2386" s="1"/>
+      <c r="FX2386" s="1"/>
+      <c r="GB2386" s="1"/>
+      <c r="GD2386" s="1"/>
+      <c r="GH2386" s="1"/>
+      <c r="GP2386" s="1"/>
+      <c r="GS2386" s="1"/>
+      <c r="HJ2386" s="1"/>
+      <c r="HN2386" s="1"/>
+      <c r="HQ2386" s="1"/>
     </row>
-    <row r="2387" spans="22:225" x14ac:dyDescent="0.3">
-      <c r="V2387" s="1"/>
-      <c r="Z2387" s="1"/>
-      <c r="AA2387" s="1"/>
-      <c r="AI2387" s="1"/>
-      <c r="AV2387" s="1"/>
-      <c r="AW2387" s="1"/>
-      <c r="BE2387" s="1"/>
-      <c r="BF2387" s="1"/>
-      <c r="BI2387" s="1"/>
-      <c r="BP2387" s="1"/>
-      <c r="BQ2387" s="1"/>
-      <c r="BV2387" s="1"/>
-      <c r="CF2387" s="1"/>
-      <c r="CI2387" s="1"/>
-      <c r="CL2387" s="1"/>
-      <c r="CS2387" s="1"/>
-      <c r="CV2387" s="1"/>
-      <c r="DI2387" s="1"/>
-      <c r="DT2387" s="1"/>
-      <c r="DY2387" s="1"/>
-      <c r="EI2387" s="1"/>
-      <c r="EQ2387" s="1"/>
-      <c r="ES2387" s="1"/>
-      <c r="EV2387" s="1"/>
-      <c r="FE2387" s="1"/>
-      <c r="FF2387" s="1"/>
-      <c r="FJ2387" s="1"/>
-      <c r="FK2387" s="1"/>
-      <c r="FP2387" s="1"/>
-      <c r="FX2387" s="1"/>
-      <c r="GB2387" s="1"/>
-      <c r="GD2387" s="1"/>
-      <c r="GH2387" s="1"/>
-      <c r="GP2387" s="1"/>
-      <c r="GS2387" s="1"/>
-      <c r="HJ2387" s="1"/>
-      <c r="HN2387" s="1"/>
-      <c r="HQ2387" s="1"/>
+    <row r="2423" spans="36:101" x14ac:dyDescent="0.3">
+      <c r="AJ2423" s="1"/>
+      <c r="AR2423" s="1"/>
+      <c r="BB2423" s="1"/>
+      <c r="BO2423" s="1"/>
+      <c r="CP2423" s="1"/>
+      <c r="CQ2423" s="1"/>
+      <c r="CW2423" s="1"/>
     </row>
     <row r="2424" spans="36:101" x14ac:dyDescent="0.3">
       <c r="AJ2424" s="1"/>
       <c r="AR2424" s="1"/>
-      <c r="BB2424" s="1"/>
       <c r="BO2424" s="1"/>
       <c r="CP2424" s="1"/>
       <c r="CQ2424" s="1"/>
       <c r="CW2424" s="1"/>
     </row>
-    <row r="2425" spans="36:101" x14ac:dyDescent="0.3">
-      <c r="AJ2425" s="1"/>
-      <c r="AR2425" s="1"/>
-      <c r="BO2425" s="1"/>
-      <c r="CP2425" s="1"/>
-      <c r="CQ2425" s="1"/>
-      <c r="CW2425" s="1"/>
+    <row r="2492" spans="50:50" x14ac:dyDescent="0.3">
+      <c r="AX2492" s="1"/>
     </row>
-    <row r="2493" spans="50:50" x14ac:dyDescent="0.3">
-      <c r="AX2493" s="1"/>
+    <row r="2636" spans="36:222" x14ac:dyDescent="0.3">
+      <c r="AJ2636" s="1"/>
+      <c r="AS2636" s="1"/>
+      <c r="BF2636" s="1"/>
+      <c r="BM2636" s="1"/>
+      <c r="CJ2636" s="1"/>
+      <c r="CS2636" s="1"/>
+      <c r="DY2636" s="1"/>
+      <c r="EQ2636" s="1"/>
+      <c r="EW2636" s="1"/>
+      <c r="FX2636" s="1"/>
+      <c r="GD2636" s="1"/>
+      <c r="GP2636" s="1"/>
+      <c r="GS2636" s="1"/>
+      <c r="GY2636" s="1"/>
     </row>
-    <row r="2637" spans="36:222" x14ac:dyDescent="0.3">
-      <c r="AJ2637" s="1"/>
-      <c r="AS2637" s="1"/>
-      <c r="BF2637" s="1"/>
-      <c r="BM2637" s="1"/>
-      <c r="CJ2637" s="1"/>
-      <c r="CS2637" s="1"/>
-      <c r="DY2637" s="1"/>
-      <c r="EQ2637" s="1"/>
-      <c r="EW2637" s="1"/>
-      <c r="FX2637" s="1"/>
-      <c r="GD2637" s="1"/>
-      <c r="GP2637" s="1"/>
-      <c r="GS2637" s="1"/>
-      <c r="GY2637" s="1"/>
+    <row r="2639" spans="36:222" x14ac:dyDescent="0.3">
+      <c r="AJ2639" s="1"/>
+      <c r="AR2639" s="1"/>
+      <c r="AS2639" s="1"/>
+      <c r="BC2639" s="1"/>
+      <c r="BF2639" s="1"/>
+      <c r="BM2639" s="1"/>
+      <c r="BQ2639" s="1"/>
+      <c r="CD2639" s="1"/>
+      <c r="CJ2639" s="1"/>
+      <c r="CP2639" s="1"/>
+      <c r="CQ2639" s="1"/>
+      <c r="CS2639" s="1"/>
+      <c r="CW2639" s="1"/>
+      <c r="DY2639" s="1"/>
+      <c r="EQ2639" s="1"/>
+      <c r="EW2639" s="1"/>
+      <c r="FE2639" s="1"/>
+      <c r="GD2639" s="1"/>
+      <c r="GP2639" s="1"/>
+      <c r="GS2639" s="1"/>
+      <c r="HN2639" s="1"/>
     </row>
-    <row r="2640" spans="36:222" x14ac:dyDescent="0.3">
-      <c r="AJ2640" s="1"/>
-      <c r="AR2640" s="1"/>
-      <c r="AS2640" s="1"/>
-      <c r="BC2640" s="1"/>
-      <c r="BF2640" s="1"/>
-      <c r="BM2640" s="1"/>
-      <c r="BQ2640" s="1"/>
-      <c r="CD2640" s="1"/>
-      <c r="CJ2640" s="1"/>
-      <c r="CP2640" s="1"/>
-      <c r="CQ2640" s="1"/>
-      <c r="CS2640" s="1"/>
-      <c r="CW2640" s="1"/>
-      <c r="DY2640" s="1"/>
-      <c r="EQ2640" s="1"/>
-      <c r="EW2640" s="1"/>
-      <c r="FE2640" s="1"/>
-      <c r="GD2640" s="1"/>
-      <c r="GP2640" s="1"/>
-      <c r="GS2640" s="1"/>
-      <c r="HN2640" s="1"/>
+    <row r="2696" spans="59:59" x14ac:dyDescent="0.3">
+      <c r="BG2696" s="1"/>
     </row>
-    <row r="2697" spans="59:59" x14ac:dyDescent="0.3">
-      <c r="BG2697" s="1"/>
+    <row r="2713" spans="50:201" x14ac:dyDescent="0.3">
+      <c r="BF2713" s="1"/>
+      <c r="BM2713" s="1"/>
+      <c r="CJ2713" s="1"/>
+      <c r="DY2713" s="1"/>
+      <c r="EQ2713" s="1"/>
+      <c r="EW2713" s="1"/>
+      <c r="FX2713" s="1"/>
+      <c r="GD2713" s="1"/>
+      <c r="GP2713" s="1"/>
+      <c r="GS2713" s="1"/>
     </row>
-    <row r="2714" spans="50:201" x14ac:dyDescent="0.3">
-      <c r="BF2714" s="1"/>
-      <c r="BM2714" s="1"/>
-      <c r="CJ2714" s="1"/>
-      <c r="DY2714" s="1"/>
-      <c r="EQ2714" s="1"/>
-      <c r="EW2714" s="1"/>
-      <c r="FX2714" s="1"/>
-      <c r="GD2714" s="1"/>
-      <c r="GP2714" s="1"/>
-      <c r="GS2714" s="1"/>
+    <row r="2718" spans="50:201" x14ac:dyDescent="0.3">
+      <c r="AX2718" s="1"/>
     </row>
-    <row r="2719" spans="50:201" x14ac:dyDescent="0.3">
-      <c r="AX2719" s="1"/>
+    <row r="2720" spans="50:201" x14ac:dyDescent="0.3">
+      <c r="AX2720" s="1"/>
     </row>
-    <row r="2721" spans="50:201" x14ac:dyDescent="0.3">
-      <c r="AX2721" s="1"/>
+    <row r="2726" spans="58:201" x14ac:dyDescent="0.3">
+      <c r="BF2726" s="1"/>
+      <c r="BM2726" s="1"/>
+      <c r="CJ2726" s="1"/>
+      <c r="CS2726" s="1"/>
+      <c r="EW2726" s="1"/>
+      <c r="GD2726" s="1"/>
+      <c r="GS2726" s="1"/>
     </row>
-    <row r="2727" spans="50:201" x14ac:dyDescent="0.3">
+    <row r="2727" spans="58:201" x14ac:dyDescent="0.3">
       <c r="BF2727" s="1"/>
       <c r="BM2727" s="1"/>
       <c r="CJ2727" s="1"/>
@@ -19686,28 +19630,19 @@
       <c r="GD2727" s="1"/>
       <c r="GS2727" s="1"/>
     </row>
-    <row r="2728" spans="50:201" x14ac:dyDescent="0.3">
-      <c r="BF2728" s="1"/>
-      <c r="BM2728" s="1"/>
-      <c r="CJ2728" s="1"/>
-      <c r="CS2728" s="1"/>
-      <c r="EW2728" s="1"/>
-      <c r="GD2728" s="1"/>
-      <c r="GS2728" s="1"/>
+    <row r="2890" spans="50:50" x14ac:dyDescent="0.3">
+      <c r="AX2890" s="1"/>
     </row>
-    <row r="2891" spans="50:50" x14ac:dyDescent="0.3">
-      <c r="AX2891" s="1"/>
+    <row r="3133" spans="149:149" x14ac:dyDescent="0.3">
+      <c r="ES3133" s="1"/>
     </row>
     <row r="3134" spans="149:149" x14ac:dyDescent="0.3">
       <c r="ES3134" s="1"/>
     </row>
-    <row r="3135" spans="149:149" x14ac:dyDescent="0.3">
-      <c r="ES3135" s="1"/>
-    </row>
-    <row r="3148" spans="27:63" x14ac:dyDescent="0.3">
-      <c r="AA3148" s="1"/>
-      <c r="BG3148" s="1"/>
-      <c r="BK3148" s="1"/>
+    <row r="3147" spans="27:63" x14ac:dyDescent="0.3">
+      <c r="AA3147" s="1"/>
+      <c r="BG3147" s="1"/>
+      <c r="BK3147" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19715,9 +19650,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19867,19 +19805,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD2B8340-481F-41E0-A263-27D4BAD65984}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE3929B2-6DC5-47B0-9B4F-8A9F81EC2CC2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -19903,9 +19837,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE3929B2-6DC5-47B0-9B4F-8A9F81EC2CC2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD2B8340-481F-41E0-A263-27D4BAD65984}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>